<commit_message>
... Unifac GC 2017
</commit_message>
<xml_diff>
--- a/data/Unifac-2017.xlsx
+++ b/data/Unifac-2017.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\UNAL\2017\TRABAJO FINAL\Java\CAMD-nuHAEA\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\UNAL\2017\TRABAJO FINAL\Java\CAMD-nuHAEA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" xr2:uid="{69F665D0-AFCD-4318-ABBD-3D289C6C1BA1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1" xr2:uid="{69F665D0-AFCD-4318-ABBD-3D289C6C1BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="UNIFAC-DORTMUND-Interactions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="171">
   <si>
     <t>i</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Subgroup Name</t>
-  </si>
-  <si>
-    <t>Main Group No.</t>
   </si>
   <si>
     <t>Main Group Name</t>
@@ -541,10 +538,7 @@
     <t>C5H4N+</t>
   </si>
   <si>
-    <t>Main Group No</t>
-  </si>
-  <si>
-    <t/>
+    <t>Main Group</t>
   </si>
 </sst>
 </file>
@@ -1003,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654D54EF-150D-49A8-8961-B65478CD1410}">
   <dimension ref="A1:H757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A716" workbookViewId="0">
-      <selection activeCell="K725" sqref="K725"/>
+    <sheetView topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="C694" sqref="C694"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17753,48 +17747,46 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE23D229-E5EF-41E6-84E9-F397290C260A}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -17802,91 +17794,79 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="F2" s="2">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="G2" s="2">
         <v>1.0608</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>172</v>
+      <c r="B3" s="2">
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="F3" s="2">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="G3" s="2">
         <v>0.70809999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>172</v>
+      <c r="B4" s="2">
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="F4" s="2">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="G4" s="2">
         <v>0.35539999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>172</v>
+      <c r="B5" s="2">
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0.63249999999999995</v>
       </c>
       <c r="F5" s="2">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="G5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -17894,91 +17874,79 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>1.2831999999999999</v>
       </c>
       <c r="F6" s="2">
-        <v>1.2831999999999999</v>
-      </c>
-      <c r="G6" s="2">
         <v>1.6015999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>172</v>
+      <c r="B7" s="2">
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>1.2831999999999999</v>
       </c>
       <c r="F7" s="2">
-        <v>1.2831999999999999</v>
-      </c>
-      <c r="G7" s="2">
         <v>1.2488999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>172</v>
+      <c r="B8" s="2">
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>1.2831999999999999</v>
       </c>
       <c r="F8" s="2">
-        <v>1.2831999999999999</v>
-      </c>
-      <c r="G8" s="2">
         <v>1.2488999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>172</v>
+      <c r="B9" s="2">
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>1.2831999999999999</v>
       </c>
       <c r="F9" s="2">
-        <v>1.2831999999999999</v>
-      </c>
-      <c r="G9" s="2">
         <v>0.8962</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -17986,45 +17954,39 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2">
-        <v>3</v>
+        <v>0.37630000000000002</v>
       </c>
       <c r="F10" s="2">
-        <v>0.37630000000000002</v>
-      </c>
-      <c r="G10" s="2">
         <v>0.43209999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>172</v>
+      <c r="B11" s="2">
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>0.37630000000000002</v>
       </c>
       <c r="F11" s="2">
-        <v>0.37630000000000002</v>
-      </c>
-      <c r="G11" s="2">
         <v>0.21129999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -18032,68 +17994,59 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>4</v>
+        <v>0.91</v>
       </c>
       <c r="F12" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="G12" s="2">
         <v>0.94899999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>172</v>
+      <c r="B13" s="2">
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2">
-        <v>4</v>
+        <v>0.91</v>
       </c>
       <c r="F13" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="G13" s="2">
         <v>0.79620000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>172</v>
+      <c r="B14" s="2">
+        <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E14" s="2">
-        <v>4</v>
+        <v>0.91</v>
       </c>
       <c r="F14" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="G14" s="2">
         <v>0.37690000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -18101,22 +18054,19 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2">
-        <v>5</v>
+        <v>1.2302</v>
       </c>
       <c r="F15" s="2">
-        <v>1.2302</v>
-      </c>
-      <c r="G15" s="2">
         <v>0.89270000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -18124,22 +18074,19 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2">
-        <v>6</v>
+        <v>0.85850000000000004</v>
       </c>
       <c r="F16" s="2">
-        <v>0.85850000000000004</v>
-      </c>
-      <c r="G16" s="2">
         <v>0.99380000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -18147,22 +18094,19 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2">
-        <v>7</v>
+        <v>1.7334000000000001</v>
       </c>
       <c r="F17" s="2">
-        <v>1.7334000000000001</v>
-      </c>
-      <c r="G17" s="2">
         <v>2.4561000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -18170,22 +18114,19 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="2">
-        <v>8</v>
+        <v>1.08</v>
       </c>
       <c r="F18" s="2">
-        <v>1.08</v>
-      </c>
-      <c r="G18" s="2">
         <v>0.97499999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -18193,45 +18134,39 @@
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2">
-        <v>9</v>
+        <v>1.7048000000000001</v>
       </c>
       <c r="F19" s="2">
-        <v>1.7048000000000001</v>
-      </c>
-      <c r="G19" s="2">
         <v>1.67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>172</v>
+      <c r="B20" s="2">
+        <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="2">
-        <v>9</v>
+        <v>1.7048000000000001</v>
       </c>
       <c r="F20" s="2">
-        <v>1.7048000000000001</v>
-      </c>
-      <c r="G20" s="2">
         <v>1.5542</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -18239,22 +18174,19 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="2">
-        <v>10</v>
+        <v>0.71730000000000005</v>
       </c>
       <c r="F21" s="2">
-        <v>0.71730000000000005</v>
-      </c>
-      <c r="G21" s="2">
         <v>0.77100000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -18262,45 +18194,39 @@
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="2">
-        <v>11</v>
+        <v>1.27</v>
       </c>
       <c r="F22" s="2">
-        <v>1.27</v>
-      </c>
-      <c r="G22" s="2">
         <v>1.6286</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>172</v>
+      <c r="B23" s="2">
+        <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E23" s="2">
-        <v>11</v>
+        <v>1.27</v>
       </c>
       <c r="F23" s="2">
-        <v>1.27</v>
-      </c>
-      <c r="G23" s="2">
         <v>1.4228000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -18308,22 +18234,19 @@
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="2">
-        <v>12</v>
+        <v>1.9</v>
       </c>
       <c r="F24" s="2">
-        <v>1.9</v>
-      </c>
-      <c r="G24" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -18331,2341 +18254,2035 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="2">
-        <v>13</v>
+        <v>1.1434</v>
       </c>
       <c r="F25" s="2">
-        <v>1.1434</v>
-      </c>
-      <c r="G25" s="2">
         <v>1.6022000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>172</v>
+      <c r="B26" s="2">
+        <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2">
-        <v>13</v>
+        <v>1.1434</v>
       </c>
       <c r="F26" s="2">
-        <v>1.1434</v>
-      </c>
-      <c r="G26" s="2">
         <v>1.2495000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>172</v>
+      <c r="B27" s="2">
+        <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="2">
-        <v>13</v>
+        <v>1.1434</v>
       </c>
       <c r="F27" s="2">
-        <v>1.1434</v>
-      </c>
-      <c r="G27" s="2">
         <v>0.89680000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="2">
-        <v>43</v>
+        <v>1.7022999999999999</v>
       </c>
       <c r="F28" s="2">
-        <v>1.7022999999999999</v>
-      </c>
-      <c r="G28" s="2">
         <v>1.8784000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="2">
-        <v>14</v>
+        <v>1.6607000000000001</v>
       </c>
       <c r="F29" s="2">
-        <v>1.6607000000000001</v>
-      </c>
-      <c r="G29" s="2">
         <v>1.6903999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>172</v>
+      <c r="B30" s="2">
+        <v>14</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" s="2">
-        <v>14</v>
+        <v>1.6607000000000001</v>
       </c>
       <c r="F30" s="2">
-        <v>1.6607000000000001</v>
-      </c>
-      <c r="G30" s="2">
         <v>1.3376999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>172</v>
+      <c r="B31" s="2">
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E31" s="2">
-        <v>14</v>
+        <v>1.6607000000000001</v>
       </c>
       <c r="F31" s="2">
-        <v>1.6607000000000001</v>
-      </c>
-      <c r="G31" s="2">
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="2">
-        <v>15</v>
+        <v>1.3680000000000001</v>
       </c>
       <c r="F32" s="2">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="G32" s="2">
         <v>1.4332</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>172</v>
+      <c r="B33" s="2">
+        <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="2">
-        <v>15</v>
+        <v>1.3680000000000001</v>
       </c>
       <c r="F33" s="2">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="G33" s="2">
         <v>1.0805</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>172</v>
+      <c r="B34" s="2">
+        <v>15</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="E34" s="2">
-        <v>15</v>
+        <v>1.3680000000000001</v>
       </c>
       <c r="F34" s="2">
-        <v>1.3680000000000001</v>
-      </c>
-      <c r="G34" s="2">
         <v>0.7278</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="2">
-        <v>16</v>
+        <v>1.0746</v>
       </c>
       <c r="F35" s="2">
-        <v>1.0746</v>
-      </c>
-      <c r="G35" s="2">
         <v>1.1759999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>172</v>
+      <c r="B36" s="2">
+        <v>16</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="E36" s="2">
-        <v>16</v>
+        <v>1.0746</v>
       </c>
       <c r="F36" s="2">
-        <v>1.0746</v>
-      </c>
-      <c r="G36" s="2">
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="2">
-        <v>17</v>
+        <v>1.1849000000000001</v>
       </c>
       <c r="F37" s="2">
-        <v>1.1849000000000001</v>
-      </c>
-      <c r="G37" s="2">
         <v>0.80669999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2">
-        <v>18</v>
+        <v>1.4578</v>
       </c>
       <c r="F38" s="2">
-        <v>1.4578</v>
-      </c>
-      <c r="G38" s="2">
         <v>0.9022</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>172</v>
+      <c r="B39" s="2">
+        <v>18</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E39" s="2">
-        <v>18</v>
+        <v>1.2393000000000001</v>
       </c>
       <c r="F39" s="2">
-        <v>1.2393000000000001</v>
-      </c>
-      <c r="G39" s="2">
         <v>0.63300000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>172</v>
+      <c r="B40" s="2">
+        <v>18</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="2">
-        <v>18</v>
+        <v>1.0730999999999999</v>
       </c>
       <c r="F40" s="2">
-        <v>1.0730999999999999</v>
-      </c>
-      <c r="G40" s="2">
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E41" s="2">
-        <v>19</v>
+        <v>1.5575000000000001</v>
       </c>
       <c r="F41" s="2">
-        <v>1.5575000000000001</v>
-      </c>
-      <c r="G41" s="2">
         <v>1.5193000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>172</v>
+      <c r="B42" s="2">
+        <v>19</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E42" s="2">
-        <v>19</v>
+        <v>1.5575000000000001</v>
       </c>
       <c r="F42" s="2">
-        <v>1.5575000000000001</v>
-      </c>
-      <c r="G42" s="2">
         <v>1.1666000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E43" s="2">
-        <v>20</v>
+        <v>0.8</v>
       </c>
       <c r="F43" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="G43" s="2">
         <v>0.92149999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E44" s="2">
-        <v>44</v>
+        <v>0.8</v>
       </c>
       <c r="F44" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="G44" s="2">
         <v>1.2742</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E45" s="2">
-        <v>21</v>
+        <v>0.9919</v>
       </c>
       <c r="F45" s="2">
-        <v>0.9919</v>
-      </c>
-      <c r="G45" s="2">
         <v>1.3653999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>172</v>
+      <c r="B46" s="2">
+        <v>21</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="E46" s="2">
-        <v>21</v>
+        <v>0.9919</v>
       </c>
       <c r="F46" s="2">
-        <v>0.9919</v>
-      </c>
-      <c r="G46" s="2">
         <v>1.0126999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>172</v>
+      <c r="B47" s="2">
+        <v>21</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E47" s="2">
-        <v>21</v>
+        <v>0.9919</v>
       </c>
       <c r="F47" s="2">
-        <v>0.9919</v>
-      </c>
-      <c r="G47" s="2">
         <v>0.66</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E48" s="2">
-        <v>22</v>
+        <v>1.8</v>
       </c>
       <c r="F48" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="G48" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>172</v>
+      <c r="B49" s="2">
+        <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E49" s="2">
-        <v>22</v>
+        <v>1.8</v>
       </c>
       <c r="F49" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="G49" s="2">
         <v>2.1473</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>172</v>
+      <c r="B50" s="2">
+        <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" s="2">
-        <v>22</v>
+        <v>1.8</v>
       </c>
       <c r="F50" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="G50" s="2">
         <v>1.7946</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E51" s="2">
-        <v>45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="F51" s="2">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="G51" s="2">
         <v>2.8912</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E52" s="2">
-        <v>23</v>
+        <v>2.65</v>
       </c>
       <c r="F52" s="2">
-        <v>2.65</v>
-      </c>
-      <c r="G52" s="2">
         <v>2.3778000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="2">
-        <v>24</v>
+        <v>2.6179999999999999</v>
       </c>
       <c r="F53" s="2">
-        <v>2.6179999999999999</v>
-      </c>
-      <c r="G53" s="2">
         <v>3.1836000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="2">
-        <v>25</v>
+        <v>0.53649999999999998</v>
       </c>
       <c r="F54" s="2">
-        <v>0.53649999999999998</v>
-      </c>
-      <c r="G54" s="2">
         <v>0.31769999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E55" s="2">
-        <v>26</v>
+        <v>2.6440000000000001</v>
       </c>
       <c r="F55" s="2">
-        <v>2.6440000000000001</v>
-      </c>
-      <c r="G55" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>172</v>
+      <c r="B56" s="2">
+        <v>26</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E56" s="2">
-        <v>26</v>
+        <v>2.5</v>
       </c>
       <c r="F56" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="G56" s="2">
         <v>2.3039999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>172</v>
+      <c r="B57" s="2">
+        <v>26</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E57" s="2">
-        <v>26</v>
+        <v>2.887</v>
       </c>
       <c r="F57" s="2">
-        <v>2.887</v>
-      </c>
-      <c r="G57" s="2">
         <v>2.2410000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E58" s="2">
-        <v>27</v>
+        <v>0.46560000000000001</v>
       </c>
       <c r="F58" s="2">
-        <v>0.46560000000000001</v>
-      </c>
-      <c r="G58" s="2">
         <v>0.3589</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E59" s="2">
-        <v>28</v>
+        <v>1.24</v>
       </c>
       <c r="F59" s="2">
-        <v>1.24</v>
-      </c>
-      <c r="G59" s="2">
         <v>1.0680000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E60" s="2">
-        <v>29</v>
+        <v>1.2889999999999999</v>
       </c>
       <c r="F60" s="2">
-        <v>1.2889999999999999</v>
-      </c>
-      <c r="G60" s="2">
         <v>1.762</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>172</v>
+      <c r="B61" s="2">
+        <v>29</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="E61" s="2">
-        <v>29</v>
+        <v>1.5349999999999999</v>
       </c>
       <c r="F61" s="2">
-        <v>1.5349999999999999</v>
-      </c>
-      <c r="G61" s="2">
         <v>1.3160000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E62" s="2">
-        <v>30</v>
+        <v>1.2989999999999999</v>
       </c>
       <c r="F62" s="2">
-        <v>1.2989999999999999</v>
-      </c>
-      <c r="G62" s="2">
         <v>1.2889999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E63" s="2">
-        <v>31</v>
+        <v>2.0880000000000001</v>
       </c>
       <c r="F63" s="2">
-        <v>2.0880000000000001</v>
-      </c>
-      <c r="G63" s="2">
         <v>2.4</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E64" s="2">
-        <v>32</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="F64" s="2">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G64" s="2">
         <v>0.91690000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="B65" s="2">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E65" s="2">
-        <v>33</v>
+        <v>1.2090000000000001</v>
       </c>
       <c r="F65" s="2">
-        <v>1.2090000000000001</v>
-      </c>
-      <c r="G65" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E66" s="2">
-        <v>34</v>
+        <v>0.9214</v>
       </c>
       <c r="F66" s="2">
-        <v>0.9214</v>
-      </c>
-      <c r="G66" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>172</v>
+      <c r="B67" s="2">
+        <v>34</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E67" s="2">
-        <v>34</v>
+        <v>1.3029999999999999</v>
       </c>
       <c r="F67" s="2">
-        <v>1.3029999999999999</v>
-      </c>
-      <c r="G67" s="2">
         <v>1.1319999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E68" s="2">
-        <v>35</v>
+        <v>3.6</v>
       </c>
       <c r="F68" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="G68" s="2">
         <v>2.6920000000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E69" s="2">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="F69" s="2">
-        <v>1</v>
-      </c>
-      <c r="G69" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E70" s="2">
-        <v>37</v>
+        <v>0.52290000000000003</v>
       </c>
       <c r="F70" s="2">
-        <v>0.52290000000000003</v>
-      </c>
-      <c r="G70" s="2">
         <v>0.73909999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E71" s="2">
-        <v>2</v>
+        <v>1.2831999999999999</v>
       </c>
       <c r="F71" s="2">
-        <v>1.2831999999999999</v>
-      </c>
-      <c r="G71" s="2">
         <v>0.4582</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E72" s="2">
-        <v>38</v>
+        <v>0.88139999999999996</v>
       </c>
       <c r="F72" s="2">
-        <v>0.88139999999999996</v>
-      </c>
-      <c r="G72" s="2">
         <v>0.72689999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" s="2">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E73" s="2">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F73" s="2">
-        <v>2</v>
-      </c>
-      <c r="G73" s="2">
         <v>2.093</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>172</v>
+      <c r="B74" s="2">
+        <v>39</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E74" s="2">
-        <v>39</v>
+        <v>2.3809999999999998</v>
       </c>
       <c r="F74" s="2">
-        <v>2.3809999999999998</v>
-      </c>
-      <c r="G74" s="2">
         <v>1.522</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
       <c r="B75" s="2">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E75" s="2">
-        <v>40</v>
+        <v>1.284</v>
       </c>
       <c r="F75" s="2">
-        <v>1.284</v>
-      </c>
-      <c r="G75" s="2">
         <v>1.266</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>172</v>
+      <c r="B76" s="2">
+        <v>40</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E76" s="2">
-        <v>40</v>
+        <v>1.284</v>
       </c>
       <c r="F76" s="2">
-        <v>1.284</v>
-      </c>
-      <c r="G76" s="2">
         <v>1.0980000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>172</v>
+      <c r="B77" s="2">
+        <v>40</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="E77" s="2">
-        <v>40</v>
+        <v>0.82150000000000001</v>
       </c>
       <c r="F77" s="2">
-        <v>0.82150000000000001</v>
-      </c>
-      <c r="G77" s="2">
         <v>0.51349999999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E78" s="2">
-        <v>41</v>
+        <v>1.6</v>
       </c>
       <c r="F78" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="G78" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" s="2">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E79" s="2">
-        <v>42</v>
+        <v>0.71360000000000001</v>
       </c>
       <c r="F79" s="2">
-        <v>0.71360000000000001</v>
-      </c>
-      <c r="G79" s="2">
         <v>0.86350000000000005</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>172</v>
+      <c r="B80" s="2">
+        <v>42</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E80" s="2">
-        <v>42</v>
+        <v>0.34789999999999999</v>
       </c>
       <c r="F80" s="2">
-        <v>0.34789999999999999</v>
-      </c>
-      <c r="G80" s="2">
         <v>0.1071</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>172</v>
+      <c r="B81" s="2">
+        <v>42</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E81" s="2">
-        <v>42</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="F81" s="2">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="G81" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
       <c r="B82" s="2">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E82" s="2">
-        <v>5</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="F82" s="2">
-        <v>1.0629999999999999</v>
-      </c>
-      <c r="G82" s="2">
         <v>0.86629999999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>172</v>
+      <c r="B83" s="2">
+        <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E83" s="2">
-        <v>5</v>
+        <v>0.6895</v>
       </c>
       <c r="F83" s="2">
-        <v>0.6895</v>
-      </c>
-      <c r="G83" s="2">
         <v>0.83450000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
       <c r="B84" s="2">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E84" s="2">
-        <v>43</v>
+        <v>1.4046000000000001</v>
       </c>
       <c r="F84" s="2">
-        <v>1.4046000000000001</v>
-      </c>
-      <c r="G84" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>172</v>
+      <c r="B85" s="2">
+        <v>43</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E85" s="2">
-        <v>43</v>
+        <v>1.0412999999999999</v>
       </c>
       <c r="F85" s="2">
-        <v>1.0412999999999999</v>
-      </c>
-      <c r="G85" s="2">
         <v>1.0116000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="B86" s="2">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E86" s="2">
-        <v>14</v>
+        <v>1.6607000000000001</v>
       </c>
       <c r="F86" s="2">
-        <v>1.6607000000000001</v>
-      </c>
-      <c r="G86" s="2">
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
       <c r="B87" s="2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E87" s="2">
-        <v>46</v>
+        <v>3.9809999999999999</v>
       </c>
       <c r="F87" s="2">
-        <v>3.9809999999999999</v>
-      </c>
-      <c r="G87" s="2">
         <v>3.2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>172</v>
+      <c r="B88" s="2">
+        <v>46</v>
       </c>
       <c r="C88" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="E88" s="2">
-        <v>46</v>
+        <v>3.7543000000000002</v>
       </c>
       <c r="F88" s="2">
-        <v>3.7543000000000002</v>
-      </c>
-      <c r="G88" s="2">
         <v>2.8919999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>172</v>
+      <c r="B89" s="2">
+        <v>46</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E89" s="2">
-        <v>46</v>
+        <v>3.5268000000000002</v>
       </c>
       <c r="F89" s="2">
-        <v>3.5268000000000002</v>
-      </c>
-      <c r="G89" s="2">
         <v>2.58</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>172</v>
+      <c r="B90" s="2">
+        <v>46</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E90" s="2">
-        <v>46</v>
+        <v>3.2993999999999999</v>
       </c>
       <c r="F90" s="2">
-        <v>3.2993999999999999</v>
-      </c>
-      <c r="G90" s="2">
         <v>2.3519999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>91</v>
       </c>
       <c r="B91" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E91" s="2">
-        <v>47</v>
+        <v>1.4515</v>
       </c>
       <c r="F91" s="2">
-        <v>1.4515</v>
-      </c>
-      <c r="G91" s="2">
         <v>1.248</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>92</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>172</v>
+      <c r="B92" s="2">
+        <v>47</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E92" s="2">
-        <v>47</v>
+        <v>1.5</v>
       </c>
       <c r="F92" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G92" s="2">
         <v>1.08</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>93</v>
       </c>
       <c r="B93" s="2">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E93" s="2">
-        <v>49</v>
+        <v>2.4617</v>
       </c>
       <c r="F93" s="2">
-        <v>2.4617</v>
-      </c>
-      <c r="G93" s="2">
         <v>2.1920000000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>94</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>172</v>
+      <c r="B94" s="2">
+        <v>49</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="E94" s="2">
-        <v>49</v>
+        <v>2.4617</v>
       </c>
       <c r="F94" s="2">
-        <v>2.4617</v>
-      </c>
-      <c r="G94" s="2">
         <v>1.8420000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>100</v>
       </c>
       <c r="B95" s="2">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E95" s="2">
-        <v>47</v>
+        <v>1.5</v>
       </c>
       <c r="F95" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G95" s="2">
         <v>1.08</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>101</v>
       </c>
       <c r="B96" s="2">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E96" s="2">
-        <v>48</v>
+        <v>2.4748000000000001</v>
       </c>
       <c r="F96" s="2">
-        <v>2.4748000000000001</v>
-      </c>
-      <c r="G96" s="2">
         <v>1.9642999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>102</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>172</v>
+      <c r="B97" s="2">
+        <v>48</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="E97" s="2">
-        <v>48</v>
+        <v>2.2738999999999998</v>
       </c>
       <c r="F97" s="2">
-        <v>2.2738999999999998</v>
-      </c>
-      <c r="G97" s="2">
         <v>1.5753999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>103</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>172</v>
+      <c r="B98" s="2">
+        <v>48</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E98" s="2">
-        <v>48</v>
+        <v>2.0767000000000002</v>
       </c>
       <c r="F98" s="2">
-        <v>2.0767000000000002</v>
-      </c>
-      <c r="G98" s="2">
         <v>1.1866000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>104</v>
       </c>
       <c r="B99" s="2">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E99" s="2">
-        <v>52</v>
+        <v>1.7943</v>
       </c>
       <c r="F99" s="2">
-        <v>1.7943</v>
-      </c>
-      <c r="G99" s="2">
         <v>1.34</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>105</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>172</v>
+      <c r="B100" s="2">
+        <v>52</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="E100" s="2">
-        <v>52</v>
+        <v>1.6282000000000001</v>
       </c>
       <c r="F100" s="2">
-        <v>1.6282000000000001</v>
-      </c>
-      <c r="G100" s="2">
         <v>1.06</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>106</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>172</v>
+      <c r="B101" s="2">
+        <v>52</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E101" s="2">
-        <v>52</v>
+        <v>1.4621</v>
       </c>
       <c r="F101" s="2">
-        <v>1.4621</v>
-      </c>
-      <c r="G101" s="2">
         <v>0.78</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>107</v>
       </c>
       <c r="B102" s="2">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E102" s="2">
-        <v>53</v>
+        <v>1.3601000000000001</v>
       </c>
       <c r="F102" s="2">
-        <v>1.3601000000000001</v>
-      </c>
-      <c r="G102" s="2">
         <v>1.8030999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>108</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>172</v>
+      <c r="B103" s="2">
+        <v>53</v>
       </c>
       <c r="C103" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="E103" s="2">
-        <v>53</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="F103" s="2">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="G103" s="2">
         <v>0.34179999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>109</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>172</v>
+      <c r="B104" s="2">
+        <v>53</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E104" s="2">
-        <v>53</v>
+        <v>0.91039999999999999</v>
       </c>
       <c r="F104" s="2">
-        <v>0.91039999999999999</v>
-      </c>
-      <c r="G104" s="2">
         <v>0.65380000000000005</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>110</v>
       </c>
       <c r="B105" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E105" s="2">
-        <v>56</v>
+        <v>2.6869999999999998</v>
       </c>
       <c r="F105" s="2">
-        <v>2.6869999999999998</v>
-      </c>
-      <c r="G105" s="2">
         <v>2.12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>111</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>172</v>
+      <c r="B106" s="2">
+        <v>56</v>
       </c>
       <c r="C106" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="E106" s="2">
-        <v>56</v>
+        <v>2.46</v>
       </c>
       <c r="F106" s="2">
-        <v>2.46</v>
-      </c>
-      <c r="G106" s="2">
         <v>1.8080000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>112</v>
       </c>
       <c r="B107" s="2">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E107" s="2">
-        <v>55</v>
+        <v>2.42</v>
       </c>
       <c r="F107" s="2">
-        <v>2.42</v>
-      </c>
-      <c r="G107" s="2">
         <v>2.4975999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>113</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>172</v>
+      <c r="B108" s="2">
+        <v>55</v>
       </c>
       <c r="C108" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D108" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E108" s="2">
-        <v>55</v>
+        <v>2.42</v>
       </c>
       <c r="F108" s="2">
-        <v>2.42</v>
-      </c>
-      <c r="G108" s="2">
         <v>2.0017999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>114</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>172</v>
+      <c r="B109" s="2">
+        <v>55</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E109" s="2">
-        <v>55</v>
+        <v>2.42</v>
       </c>
       <c r="F109" s="2">
-        <v>2.42</v>
-      </c>
-      <c r="G109" s="2">
         <v>2.2496999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>119</v>
       </c>
       <c r="B110" s="2">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E110" s="2">
-        <v>53</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="F110" s="2">
-        <v>1.0629999999999999</v>
-      </c>
-      <c r="G110" s="2">
         <v>1.123</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>122</v>
       </c>
       <c r="B111" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E111" s="2">
-        <v>61</v>
+        <v>1.613</v>
       </c>
       <c r="F111" s="2">
-        <v>1.613</v>
-      </c>
-      <c r="G111" s="2">
         <v>1.3680000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>123</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>172</v>
+      <c r="B112" s="2">
+        <v>61</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E112" s="2">
-        <v>61</v>
+        <v>1.3863000000000001</v>
       </c>
       <c r="F112" s="2">
-        <v>1.3863000000000001</v>
-      </c>
-      <c r="G112" s="2">
         <v>1.06</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>124</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>172</v>
+      <c r="B113" s="2">
+        <v>61</v>
       </c>
       <c r="C113" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="E113" s="2">
-        <v>61</v>
+        <v>1.1589</v>
       </c>
       <c r="F113" s="2">
-        <v>1.1589</v>
-      </c>
-      <c r="G113" s="2">
         <v>0.748</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>153</v>
       </c>
       <c r="B114" s="2">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E114" s="2">
-        <v>53</v>
+        <v>0.91039999999999999</v>
       </c>
       <c r="F114" s="2">
-        <v>0.91039999999999999</v>
-      </c>
-      <c r="G114" s="2">
         <v>0.65380000000000005</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>178</v>
       </c>
       <c r="B115" s="2">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E115" s="2">
-        <v>84</v>
+        <v>1.3662000000000001</v>
       </c>
       <c r="F115" s="2">
-        <v>1.3662000000000001</v>
-      </c>
-      <c r="G115" s="2">
         <v>0.67969999999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>179</v>
       </c>
       <c r="B116" s="2">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E116" s="2">
-        <v>85</v>
+        <v>5.6210000000000004</v>
       </c>
       <c r="F116" s="2">
-        <v>5.6210000000000004</v>
-      </c>
-      <c r="G116" s="2">
         <v>5.9462999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>184</v>
       </c>
       <c r="B117" s="2">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E117" s="2">
-        <v>84</v>
+        <v>1.843</v>
       </c>
       <c r="F117" s="2">
-        <v>1.843</v>
-      </c>
-      <c r="G117" s="2">
         <v>1.6997</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>189</v>
       </c>
       <c r="B118" s="2">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E118" s="2">
-        <v>87</v>
+        <v>2.7867000000000002</v>
       </c>
       <c r="F118" s="2">
-        <v>2.7867000000000002</v>
-      </c>
-      <c r="G118" s="2">
         <v>2.7723</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>195</v>
       </c>
       <c r="B119" s="2">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E119" s="2">
-        <v>89</v>
+        <v>3.9628000000000001</v>
       </c>
       <c r="F119" s="2">
-        <v>3.9628000000000001</v>
-      </c>
-      <c r="G119" s="2">
         <v>0.62139999999999995</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>196</v>
       </c>
       <c r="B120" s="2">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E120" s="2">
-        <v>90</v>
+        <v>2.1093999999999999</v>
       </c>
       <c r="F120" s="2">
-        <v>2.1093999999999999</v>
-      </c>
-      <c r="G120" s="2">
         <v>2.5106000000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>197</v>
       </c>
       <c r="B121" s="2">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E121" s="2">
-        <v>91</v>
+        <v>3.371</v>
       </c>
       <c r="F121" s="2">
-        <v>3.371</v>
-      </c>
-      <c r="G121" s="2">
         <v>2.0001000000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>201</v>
       </c>
-      <c r="B122" s="2">
-        <v>69</v>
+      <c r="B122" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G122" s="2">
+      <c r="F122" s="2">
         <v>2.2440000000000002</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>209</v>
       </c>
       <c r="B123" s="2">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E123" s="2">
-        <v>98</v>
+        <v>0.99029999999999996</v>
       </c>
       <c r="F123" s="2">
-        <v>0.99029999999999996</v>
-      </c>
-      <c r="G123" s="2">
         <v>3.5249000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>210</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>172</v>
+      <c r="B124" s="2">
+        <v>98</v>
       </c>
       <c r="C124" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="E124" s="2">
-        <v>98</v>
+        <v>1.5653999999999999</v>
       </c>
       <c r="F124" s="2">
-        <v>1.5653999999999999</v>
-      </c>
-      <c r="G124" s="2">
         <v>3.8075999999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>211</v>
       </c>
       <c r="B125" s="2">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E125" s="2">
-        <v>99</v>
+        <v>3.8182999999999998</v>
       </c>
       <c r="F125" s="2">
-        <v>3.8182999999999998</v>
-      </c>
-      <c r="G125" s="2">
         <v>3.6017999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>220</v>
       </c>
       <c r="B126" s="2">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E126" s="2">
-        <v>90</v>
+        <v>2.4872999999999998</v>
       </c>
       <c r="F126" s="2">
-        <v>2.4872999999999998</v>
-      </c>
-      <c r="G126" s="2">
         <v>2.4457</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Second order contributions GC 2017
</commit_message>
<xml_diff>
--- a/data/Unifac-2017.xlsx
+++ b/data/Unifac-2017.xlsx
@@ -17749,8 +17749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE23D229-E5EF-41E6-84E9-F397290C260A}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>